<commit_message>
Changed HTML and CSS to fit aesthetic of brief
Basic setup for functionality added
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -153,18 +153,12 @@
     <t>Method of sending emails can vary (could use php but not in scope of assignment)</t>
   </si>
   <si>
-    <t>will use php as a last resort (since I don’t really know it), but will look for various solutions</t>
-  </si>
-  <si>
     <t>UX Guide not avalible :0</t>
   </si>
   <si>
     <t>Going to use HTML forms instead of individual elements in a div</t>
   </si>
   <si>
-    <t>Checking every input at runtime seems excessive, but will add event listners at all input fields.</t>
-  </si>
-  <si>
     <t>Test data will need to conform, so must use a fake number &amp; test multiple types</t>
   </si>
   <si>
@@ -186,23 +180,140 @@
     <t>Will only use valid test data to send email.</t>
   </si>
   <si>
-    <t>Validity would be checked during user input to adhere with CTO case ID 9</t>
-  </si>
-  <si>
-    <t>Validity would be checked during user input to adhere with CTO case ID 10</t>
-  </si>
-  <si>
-    <t>Validity would be checked during user input to adhere with CTO case ID 11</t>
-  </si>
-  <si>
     <t>Need to relearn what the algorithm is lol</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>front end test code loads correctly</t>
+  </si>
+  <si>
+    <t>Webpage loads basic HTML/CSS/JS elements</t>
+  </si>
+  <si>
+    <t>console.log hello world + css aqua</t>
+  </si>
+  <si>
+    <t>Link files to HTML for loading</t>
+  </si>
+  <si>
+    <t>bg color change, and console log showing correct test data</t>
+  </si>
+  <si>
+    <t>JS loaded fine, CSS body code was wrong</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Changed css to correct code, and all loads fine</t>
+  </si>
+  <si>
+    <t>Checking every input at runtime seems excessive, but will add event listners at all input fields.will show error message if input contains satan characters.</t>
+  </si>
+  <si>
+    <t>Names would just be anything from 2-20 characters long</t>
+  </si>
+  <si>
+    <t>What counts as a valid name?</t>
+  </si>
+  <si>
+    <t>Validity would be checked during user input to adhere with CTO case ID 9. Checks specifically for an @ symbol, and within the 2-20 character range</t>
+  </si>
+  <si>
+    <t>will use php as a last resort (since I don’t really know it), but will look for various solutions. EDIT: basically HTML has a built in thing for the forms, so will be using that.</t>
+  </si>
+  <si>
+    <t>Validity would be checked during user input to adhere with CTO case ID 9 + LUHN algorithm as mentioned down below</t>
+  </si>
+  <si>
+    <t>https://imgur.com/xmqq2ry</t>
+  </si>
+  <si>
+    <t>Image Proof</t>
+  </si>
+  <si>
+    <t>Font Loads as calibri, has a fixed text size and is centered horizontally</t>
+  </si>
+  <si>
+    <t>A h1 tag needs to be in place to be centered and to check the font</t>
+  </si>
+  <si>
+    <t>User Data</t>
+  </si>
+  <si>
+    <t>Change document wide css to make font correct + center it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nice text </t>
+  </si>
+  <si>
+    <t>Wasn’t actually sure what calibri looked like, and had to double check online</t>
+  </si>
+  <si>
+    <t>Looks sicko</t>
+  </si>
+  <si>
+    <t>Needs form html tags in place, inside of a div</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Form needs to be added to HTML file</t>
+  </si>
+  <si>
+    <t>Areas of for user input need to be added and interactable</t>
+  </si>
+  <si>
+    <t>input fields are labeled correctly and 1a! Can be put into all 3</t>
+  </si>
+  <si>
+    <t>Create a form with 3 input fields, labeled in the HTML document</t>
+  </si>
+  <si>
+    <t>All would be interactable and visible</t>
+  </si>
+  <si>
+    <t>https://imgur.com/lJt64tf</t>
+  </si>
+  <si>
+    <t>the div with user input form needs to match wireframe colors</t>
+  </si>
+  <si>
+    <t>Add bg in css</t>
+  </si>
+  <si>
+    <t>Background Change</t>
+  </si>
+  <si>
+    <t>Didn’t change into given color</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>https://imgur.com/2QC8t1U</t>
+  </si>
+  <si>
+    <t>https://imgur.com/vHtYIKo</t>
+  </si>
+  <si>
+    <t>Form was added fine, but formatting was weird, so needs CSS changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used an eyedropper color, which wasn’t given in brief, so changed. Also think the id name of the div was wrong </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +331,14 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -308,10 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,9 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -346,8 +463,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,173 +750,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="50.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="K1" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" s="3">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K5" r:id="rId3"/>
+    <hyperlink ref="K4" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -800,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,28 +1038,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -862,7 +1081,7 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -883,7 +1102,7 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -904,7 +1123,7 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -923,9 +1142,11 @@
       <c r="H5" s="3">
         <v>4</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="J5" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -946,7 +1167,7 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -967,7 +1188,7 @@
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -990,7 +1211,7 @@
         <v>28</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1010,10 +1231,10 @@
         <v>8</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1033,7 +1254,7 @@
         <v>9</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="3"/>
     </row>
@@ -1057,7 +1278,7 @@
         <v>33</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1077,10 +1298,10 @@
         <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1103,7 +1324,7 @@
         <v>34</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1123,10 +1344,10 @@
         <v>13</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1151,7 +1372,7 @@
         <v>36</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed HTML Post Method
title
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -375,16 +375,40 @@
     <t>nothing happened</t>
   </si>
   <si>
-    <t>Using my trusty friend google, I found out I needed to change the form action to 'mailto:email'</t>
-  </si>
-  <si>
-    <t>Sends data to an email</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>I believe my form settings are to blame</t>
+  </si>
+  <si>
+    <t>https://imgur.com/scbZorC</t>
+  </si>
+  <si>
+    <t>https://imgur.com/Zx59B0g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using my trusty friend google, I found out I needed to change the form action to 'mailto:email'. Unfortunately no data is added to the email, but I think this is an easily solvable issue with the form settings                                  </t>
+  </si>
+  <si>
+    <t>Need a PHP script to take the given data and send it to a user</t>
+  </si>
+  <si>
+    <t>Using my test email</t>
+  </si>
+  <si>
+    <t>using script from: https://html.form.guide/email-form/html-email-form/ I will make the form action send an email through PHP</t>
+  </si>
+  <si>
+    <t>Would open a new tab with my PHP Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t think this is the way to go. Apparently you need a server or client side host 'thing', and it just seems like its not in the scope, since it wasn't specifically specified. Also I have no idea what I'm doing with it.                 </t>
+  </si>
+  <si>
+    <t>Sends data to an email to be sent to user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a bit to the mailto action in HTML, that sets input as body text, but includes HTML code which isn't idea, but technically a success. I think this is something to solve with JavaScript, when I actually get there      </t>
+  </si>
+  <si>
+    <t>https://imgur.com/1Ls3ar9</t>
   </si>
 </sst>
 </file>
@@ -840,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,12 +1167,14 @@
         <v>84</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K8" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1171,16 +1197,130 @@
         <v>109</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K9" s="2"/>
       <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="14"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1191,9 +1331,12 @@
     <hyperlink ref="K6" r:id="rId5"/>
     <hyperlink ref="K7" r:id="rId6" display="https://imgur.com/help3Zf"/>
     <hyperlink ref="L7" r:id="rId7" display="https://imgur.com/a1NcJAe"/>
+    <hyperlink ref="K8" r:id="rId8"/>
+    <hyperlink ref="K9" r:id="rId9"/>
+    <hyperlink ref="K11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added event listeners to all fields
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="159">
   <si>
     <t>ID</t>
   </si>
@@ -439,6 +439,84 @@
   </si>
   <si>
     <t>When the page is in desktop (in larger views), because I am using % scaling, it will reach to the sides quite far. I don’t think this looks particularly bad, but would understand if this is something undisired in the final result</t>
+  </si>
+  <si>
+    <t>Javascript action listener should detect use of the submit button</t>
+  </si>
+  <si>
+    <t>Submit button and javascript actionlistener need to be present</t>
+  </si>
+  <si>
+    <t>console.log("HELLO :)");</t>
+  </si>
+  <si>
+    <t>After adding function, check submit button produces test data in console</t>
+  </si>
+  <si>
+    <t>hello in console</t>
+  </si>
+  <si>
+    <t>https://imgur.com/O9AQ81t</t>
+  </si>
+  <si>
+    <t>Console window epxlaining wrong syntax</t>
+  </si>
+  <si>
+    <t>https://imgur.com/GCRzhH9</t>
+  </si>
+  <si>
+    <t>Javascript action listener should detect user click input</t>
+  </si>
+  <si>
+    <t>javascript actionlistener needs to be present</t>
+  </si>
+  <si>
+    <t>Shows hello, but no functionallity.</t>
+  </si>
+  <si>
+    <t>Text loads when script loads. Believe this could be due to loading in the head, instead of body but also could be due to the way I have made the function</t>
+  </si>
+  <si>
+    <t>https://imgur.com/2cPukwi</t>
+  </si>
+  <si>
+    <t>While using an eventlistener function found online click on the screen</t>
+  </si>
+  <si>
+    <t>Produces hello in console when clicked anywhere on document</t>
+  </si>
+  <si>
+    <t>I think I was trying to incorporate one of these =&gt;, since it was what I used last time. Also code is from w3schools</t>
+  </si>
+  <si>
+    <t>After editing old  function, check submit button produces test data in console</t>
+  </si>
+  <si>
+    <t>Produces hello in console when submit button is clicked</t>
+  </si>
+  <si>
+    <t>https://imgur.com/QVmL1EK</t>
+  </si>
+  <si>
+    <t>https://imgur.com/DJJxcTA</t>
+  </si>
+  <si>
+    <t>All fields detect user input (click)</t>
+  </si>
+  <si>
+    <t>actionlisteners + html elements</t>
+  </si>
+  <si>
+    <t>Add all eventlisteners to all inputs</t>
+  </si>
+  <si>
+    <t>hello in console for each input clicked on</t>
+  </si>
+  <si>
+    <t>Used an array and looped through to add event listeners to each. Think this might need changing for code readablity, since userElement[1] isn't very descriptive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All fields produce hello when clicked </t>
   </si>
 </sst>
 </file>
@@ -897,7 +975,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,84 +1460,180 @@
       </c>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="14"/>
+      <c r="B15" s="3">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="14"/>
+      <c r="B16" s="3">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="B17" s="3">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="14"/>
+      <c r="K17" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="14"/>
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>152</v>
+      </c>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1620,9 +1794,14 @@
     <hyperlink ref="K11" r:id="rId10"/>
     <hyperlink ref="K12" r:id="rId11"/>
     <hyperlink ref="K13" r:id="rId12"/>
+    <hyperlink ref="K14" r:id="rId13"/>
+    <hyperlink ref="K15" r:id="rId14"/>
+    <hyperlink ref="K16" r:id="rId15"/>
+    <hyperlink ref="K17" r:id="rId16"/>
+    <hyperlink ref="K18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
make fields detect user input
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t xml:space="preserve">All fields produce hello when clicked </t>
+  </si>
+  <si>
+    <t>Changed array to an object with help from https://masteringjs.io/tutorials/fundamentals/foreach-object to add event listeners, while keeping code easier to read</t>
+  </si>
+  <si>
+    <t>https://imgur.com/EDmnBzc</t>
   </si>
 </sst>
 </file>
@@ -975,7 +981,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,20 +1642,40 @@
       </c>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="14"/>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1799,9 +1825,10 @@
     <hyperlink ref="K16" r:id="rId15"/>
     <hyperlink ref="K17" r:id="rId16"/>
     <hyperlink ref="K18" r:id="rId17"/>
+    <hyperlink ref="K19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added keycode check and banned keycode array for user inputs
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -372,9 +372,6 @@
     <t>nothing happened</t>
   </si>
   <si>
-    <t>I believe my form settings are to blame</t>
-  </si>
-  <si>
     <t>https://imgur.com/scbZorC</t>
   </si>
   <si>
@@ -402,9 +399,6 @@
     <t>https://imgur.com/1Ls3ar9</t>
   </si>
   <si>
-    <t>Added a bit to the mailto action in HTML, that sets input as body text, but includes HTML code which isn't idea, but technically a success. I think this is something to solve with JavaScript, when I actually get there (saving until basic framework is fully in place )</t>
-  </si>
-  <si>
     <t xml:space="preserve">Don’t think this is the way to go. Apparently you need a server or client side hosting 'thing', and  since it wasn't specifically specified this just intuitively feels wrong. Also I have no idea what I'm doing with it.                 </t>
   </si>
   <si>
@@ -523,6 +517,219 @@
   </si>
   <si>
     <t>https://imgur.com/EDmnBzc</t>
+  </si>
+  <si>
+    <t>https://imgur.com/kzrrqLH</t>
+  </si>
+  <si>
+    <t>https://imgur.com/kBHIZPq</t>
+  </si>
+  <si>
+    <t>https://imgur.com/LFvOmV8</t>
+  </si>
+  <si>
+    <t>https://imgur.com/8vWM8Ca</t>
+  </si>
+  <si>
+    <t>https://imgur.com/EKuiOEv</t>
+  </si>
+  <si>
+    <t>All fields detect all user input</t>
+  </si>
+  <si>
+    <t>Shows the last input used, but not the entire string, which will be needed for checking validity</t>
+  </si>
+  <si>
+    <t>Showed object names &amp; doesn’t respond to input events</t>
+  </si>
+  <si>
+    <t>Write test data into fields while checking console window to see if it is detecting input</t>
+  </si>
+  <si>
+    <t>shows 123 in console</t>
+  </si>
+  <si>
+    <t>Function for checking input needs to correctly corrospond to input</t>
+  </si>
+  <si>
+    <t>not responding to input, only the name of the field on loading</t>
+  </si>
+  <si>
+    <t>Need to recheck how JS actionlistener syntax is written, as I believe I was too confident in my knowledge before writing this</t>
+  </si>
+  <si>
+    <t>Hello world</t>
+  </si>
+  <si>
+    <t>shows hello world</t>
+  </si>
+  <si>
+    <t>responds to input, but doesn’t show specific input values</t>
+  </si>
+  <si>
+    <t>Need to change what the function outputs, but am on the right track.</t>
+  </si>
+  <si>
+    <t>Only shows one value, instead of whole string. This could be added to an array to be checked, but seems redundant when it should be in the field objects data</t>
+  </si>
+  <si>
+    <t>https://imgur.com/83KhElj</t>
+  </si>
+  <si>
+    <t>Now shows whole string in console of name field input, but not the others</t>
+  </si>
+  <si>
+    <t>https://imgur.com/eXQwCDl</t>
+  </si>
+  <si>
+    <t>Console shows all fields with all data (though is hard to read)</t>
+  </si>
+  <si>
+    <t>shows 123 in console for each field</t>
+  </si>
+  <si>
+    <t>Write test data into  all fields while checking console window to see if it is detecting input</t>
+  </si>
+  <si>
+    <t>Form settings need changing</t>
+  </si>
+  <si>
+    <t>Added a bit to the mailto action in HTML, that sets input as body text, but includes HTML code which isn't ideal, but technically a success. I think this is something to solve with JavaScript, when I actually get there (saving until basic framework is fully in place )</t>
+  </si>
+  <si>
+    <t>Realised this is checking event data, not object data. Will need to either loop through each object input value or hard code it in each one.</t>
+  </si>
+  <si>
+    <t>was correct :)</t>
+  </si>
+  <si>
+    <t>Streamlined code and made it better and stuff</t>
+  </si>
+  <si>
+    <t>https://imgur.com/QYkbz88</t>
+  </si>
+  <si>
+    <t>Emails Include @ and . Symbols, which are unspecified. Also not sure if there is a grammar error, as the listed printable characters are essential for SQL Injections</t>
+  </si>
+  <si>
+    <t>Will check for ascii UTF-8 Valid characters only (charcodes 32-126). Will also exclude keycodes for the characters ().:;&lt;&gt;[\]^</t>
+  </si>
+  <si>
+    <t>https://imgur.com/Oqg8LhL</t>
+  </si>
+  <si>
+    <t>ASCII Keycodes are read correctly</t>
+  </si>
+  <si>
+    <t>User input detection + keycode check function</t>
+  </si>
+  <si>
+    <t>Keycodes for 123 shown in console</t>
+  </si>
+  <si>
+    <t>Write test data into  all fields while checking console window to see if it is detecting Ascii keycodes</t>
+  </si>
+  <si>
+    <t>Shows error message</t>
+  </si>
+  <si>
+    <t>https://imgur.com/ZgFV0oQ</t>
+  </si>
+  <si>
+    <t>string characters are read correctly</t>
+  </si>
+  <si>
+    <t>Shows characters at each index of the user input fields when interacting</t>
+  </si>
+  <si>
+    <t>Now just need to convert to ascii keycodes</t>
+  </si>
+  <si>
+    <t>https://imgur.com/tLsAdYW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows each ascii keycode in </t>
+  </si>
+  <si>
+    <t>Created an array for each banned ascii character within the standard printable character range which is ().;:&lt;&gt;[\]^. I think my error in this case is just a syntax issue, but will try with the characters instead to see if my method actually works</t>
+  </si>
+  <si>
+    <t>Used CharCodeAt to get the keycode of the index. Am going to compare this to https://theasciicode.com.ar/ for the keycode refrence</t>
+  </si>
+  <si>
+    <t>https://imgur.com/ReSUVx0</t>
+  </si>
+  <si>
+    <t>ASCII Keycodes are the same as the ones used in my banned keycode array</t>
+  </si>
+  <si>
+    <t>Array of banned keycodes + input detection in each field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ().;:&lt;&gt;[\]</t>
+  </si>
+  <si>
+    <t>Write test data into a field and see if it corresponds to the data given online and in array</t>
+  </si>
+  <si>
+    <t>Keycodes Match</t>
+  </si>
+  <si>
+    <t>Done to check if the online resources matched up. I have had issues in the past of these not matching up, so this was just a double check</t>
+  </si>
+  <si>
+    <t>Convert function to one that checks and compares values to keycodes</t>
+  </si>
+  <si>
+    <t>https://imgur.com/K0YAu30</t>
+  </si>
+  <si>
+    <t>Warns you when a banned keycode is present</t>
+  </si>
+  <si>
+    <t>Surprised it worked 1st try, now will try seeing if using a keycode outside of accepted 32-126 range will produce unexpected results</t>
+  </si>
+  <si>
+    <t>12^</t>
+  </si>
+  <si>
+    <t>input test data and see if console warns of issue</t>
+  </si>
+  <si>
+    <t>Function with a for loop to detect if array elements are the same as characters in user inputs</t>
+  </si>
+  <si>
+    <t>keycodes outside of 32-126 range are console logged as bad</t>
+  </si>
+  <si>
+    <t>Function with a for loop to detect if  user inputs are outside of given range</t>
+  </si>
+  <si>
+    <t>Ç</t>
+  </si>
+  <si>
+    <t>input test data in field, and see if console admits to wrongdoings (general evilness)</t>
+  </si>
+  <si>
+    <t>console logs that input is out of range</t>
+  </si>
+  <si>
+    <t>console didn’t let me know :(</t>
+  </si>
+  <si>
+    <t>Think I need to change my if statement to be &amp;&amp;, as well as making the range tighter (is &gt; 32 &amp; &lt;127 at the moment)</t>
+  </si>
+  <si>
+    <t>https://imgur.com/9A76Mbb</t>
+  </si>
+  <si>
+    <t>The console did let me know what keycode wasn’t in the acceptable range</t>
+  </si>
+  <si>
+    <t>https://imgur.com/2CxEYA8</t>
+  </si>
+  <si>
+    <t>The ascii keycode described on the website (website was 128, instead of 199) didn’t match up to the one given by JavaScript, so either the website is wrong, or I'm using some other kind of  keycodes without realising</t>
   </si>
 </sst>
 </file>
@@ -978,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1317,7 @@
       </c>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1281,10 +1488,10 @@
         <v>83</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>111</v>
       </c>
       <c r="L8" s="13"/>
     </row>
@@ -1311,16 +1518,16 @@
         <v>108</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L9" s="13"/>
     </row>
@@ -1335,30 +1542,30 @@
         <v>104</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>108</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1381,16 +1588,16 @@
         <v>108</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="L11" s="13"/>
     </row>
@@ -1402,31 +1609,31 @@
         <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L12" s="13"/>
     </row>
@@ -1438,31 +1645,31 @@
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="K13" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L13" s="13"/>
     </row>
@@ -1474,29 +1681,29 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L14" s="13"/>
     </row>
@@ -1508,31 +1715,31 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>83</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L15" s="13"/>
     </row>
@@ -1544,31 +1751,31 @@
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L16" s="13"/>
     </row>
@@ -1580,29 +1787,29 @@
         <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L17" s="13"/>
     </row>
@@ -1614,31 +1821,31 @@
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L18" s="13"/>
     </row>
@@ -1650,161 +1857,697 @@
         <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="3">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="3">
+        <v>123</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="14"/>
+      <c r="K20" s="14" t="s">
+        <v>159</v>
+      </c>
       <c r="L20" s="13"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="3">
+        <v>123</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="14"/>
+      <c r="K21" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="14"/>
+      <c r="B22" s="3">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="3">
+        <v>123</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>161</v>
+      </c>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="14"/>
+      <c r="B23" s="3">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="14"/>
+      <c r="B24" s="3">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="3">
+        <v>123</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>163</v>
+      </c>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="14"/>
+      <c r="B25" s="3">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="3">
+        <v>123</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="L25" s="13"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="14"/>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="3">
+        <v>123</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="L26" s="13"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="14"/>
+      <c r="B27" s="3">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="3">
+        <v>123</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="3">
+        <v>123</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3">
+        <v>11</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="3">
+        <v>123</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" s="3">
+        <v>123</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>11</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3">
+        <v>11</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="13"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1826,9 +2569,24 @@
     <hyperlink ref="K17" r:id="rId16"/>
     <hyperlink ref="K18" r:id="rId17"/>
     <hyperlink ref="K19" r:id="rId18"/>
+    <hyperlink ref="K20" r:id="rId19"/>
+    <hyperlink ref="K21" r:id="rId20"/>
+    <hyperlink ref="K22" r:id="rId21"/>
+    <hyperlink ref="K23" r:id="rId22"/>
+    <hyperlink ref="K24" r:id="rId23"/>
+    <hyperlink ref="K25" r:id="rId24"/>
+    <hyperlink ref="K26" r:id="rId25"/>
+    <hyperlink ref="K27" r:id="rId26"/>
+    <hyperlink ref="K28" r:id="rId27"/>
+    <hyperlink ref="K29" r:id="rId28"/>
+    <hyperlink ref="K30" r:id="rId29"/>
+    <hyperlink ref="K31" r:id="rId30"/>
+    <hyperlink ref="K32" r:id="rId31"/>
+    <hyperlink ref="K33" r:id="rId32"/>
+    <hyperlink ref="K34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 
@@ -1836,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2202,10 +2960,14 @@
         <v>14</v>
       </c>
       <c r="H16" s="3">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added input class and removed/commented functions
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="261">
   <si>
     <t>ID</t>
   </si>
@@ -730,6 +730,99 @@
   </si>
   <si>
     <t>The ascii keycode described on the website (website was 128, instead of 199) didn’t match up to the one given by JavaScript, so either the website is wrong, or I'm using some other kind of  keycodes without realising</t>
+  </si>
+  <si>
+    <t>console logs that input is out of range but corrosponds to keycode data</t>
+  </si>
+  <si>
+    <t>https://imgur.com/BJNZBub</t>
+  </si>
+  <si>
+    <t>The corrosponding values are correct from here.</t>
+  </si>
+  <si>
+    <t>Issues arose from not realising that the online keycodes are from event values, instead of the actual ASCII keycodes, which actually were correct when being analysed by charCodeAt</t>
+  </si>
+  <si>
+    <t>https://imgur.com/wT1yL0C</t>
+  </si>
+  <si>
+    <t>keycodes out of acceptable ranges from https://www.rapidtables.com/code/text/ascii-table.html</t>
+  </si>
+  <si>
+    <t>I also managed to accidently open the mail, and found out that certain printable characters when put into the text of the email body are very odd. I believe these are escape characters so that the \ and / don’t effect the HTML. Also using https://www.toptal.com/developers/keycode, I can see that the keycodes are wildly different from what I expect, yet my code still works properly so am genuinely unsure of what is causing this issue.</t>
+  </si>
+  <si>
+    <t>The console did let me know what keycode wasn’t in the acceptable range but still gave unexpected results</t>
+  </si>
+  <si>
+    <t>https://imgur.com/NXmpKYx</t>
+  </si>
+  <si>
+    <t>Class values are visible by console for an input field</t>
+  </si>
+  <si>
+    <t>Class template for user input to hold the data for the: dom element + its value, its given name and weather its valid</t>
+  </si>
+  <si>
+    <t>"name",document.getElementsById("name")</t>
+  </si>
+  <si>
+    <t>Create a class with given parameters defined in constructor</t>
+  </si>
+  <si>
+    <t>console should log class name validity and type of DOM used</t>
+  </si>
+  <si>
+    <t>Error at the constructor peramaters given.</t>
+  </si>
+  <si>
+    <t>Believe that the document.getId should probably instead use the JSON data, however I was planning to get rid of this if the classes worked, since this data could be stored there instead</t>
+  </si>
+  <si>
+    <t>https://imgur.com/JMNknMS</t>
+  </si>
+  <si>
+    <t>Sucessfully shown correct names and document element</t>
+  </si>
+  <si>
+    <t>Isssue was bad syntax. Used to making classes in c#, which sets constructor name to be the same as the class.</t>
+  </si>
+  <si>
+    <t>Class values are visible by console for an input field while using JSON data</t>
+  </si>
+  <si>
+    <t>"name",fields.name</t>
+  </si>
+  <si>
+    <t>https://imgur.com/6rWObKq</t>
+  </si>
+  <si>
+    <t>Worked same as above</t>
+  </si>
+  <si>
+    <t>Just to check this method works</t>
+  </si>
+  <si>
+    <t>Successful addition of action listeners to class types</t>
+  </si>
+  <si>
+    <t>input class with defined input field</t>
+  </si>
+  <si>
+    <t>add event listener to a new input field class, using its _type attribute</t>
+  </si>
+  <si>
+    <t>console log works same as before adding classes (logging input text</t>
+  </si>
+  <si>
+    <t>mirrored old code perfectly and showed input text in console</t>
+  </si>
+  <si>
+    <t>Was surprised this worked, but will create an array of these classes</t>
+  </si>
+  <si>
+    <t>https://imgur.com/rgg9jOC</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,7 +2514,7 @@
       </c>
       <c r="L34" s="13"/>
     </row>
-    <row r="35" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2441,96 +2534,200 @@
         <v>222</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J35" s="3"/>
-      <c r="K35" s="14"/>
+        <v>83</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>231</v>
+      </c>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="14"/>
+      <c r="B36" s="3">
+        <v>11</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>234</v>
+      </c>
       <c r="L36" s="13"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="14"/>
+      <c r="B37" s="3">
+        <v>11</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>238</v>
+      </c>
       <c r="L37" s="13"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="14"/>
+      <c r="B38" s="3">
+        <v>11</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>246</v>
+      </c>
       <c r="L38" s="13"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="14"/>
+      <c r="B39" s="3">
+        <v>11</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>251</v>
+      </c>
       <c r="L39" s="13"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="14"/>
+      <c r="B40" s="3">
+        <v>11</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E40" s="3">
+        <v>123</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>260</v>
+      </c>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2548,6 +2745,614 @@
       <c r="J41" s="3"/>
       <c r="K41" s="14"/>
       <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="13"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="13"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="13"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="13"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="13"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="13"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="13"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="13"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="13"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="13"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="13"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="13"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="13"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="13"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="13"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="13"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="13"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="13"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="13"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="13"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="13"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="13"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="13"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="13"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="13"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="13"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="13"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="13"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="13"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="13"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="13"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2584,9 +3389,15 @@
     <hyperlink ref="K32" r:id="rId31"/>
     <hyperlink ref="K33" r:id="rId32"/>
     <hyperlink ref="K34" r:id="rId33"/>
+    <hyperlink ref="K35" r:id="rId34"/>
+    <hyperlink ref="K36" r:id="rId35"/>
+    <hyperlink ref="K37" r:id="rId36"/>
+    <hyperlink ref="K38" r:id="rId37"/>
+    <hyperlink ref="K39" r:id="rId38"/>
+    <hyperlink ref="K40" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added all proof images
</commit_message>
<xml_diff>
--- a/Spreadsheets/Tests.xlsx
+++ b/Spreadsheets/Tests.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="327">
   <si>
     <t>ID</t>
   </si>
@@ -917,9 +917,6 @@
     <t>This needs to be put inside of the class, and also was trying to read values from the old inputs object (which now has classes instead of document.getId's)</t>
   </si>
   <si>
-    <t>https://imgur.com/undefined</t>
-  </si>
-  <si>
     <t>successfully logged the keycodes, same as previously</t>
   </si>
   <si>
@@ -927,6 +924,126 @@
   </si>
   <si>
     <t>Had to restructure the code a bit, and put the invalid keys within the ascii check method.</t>
+  </si>
+  <si>
+    <t>https://imgur.com/rECWBpZ</t>
+  </si>
+  <si>
+    <t>https://imgur.com/rHMoAGD</t>
+  </si>
+  <si>
+    <t>https://imgur.com/eQ203V1</t>
+  </si>
+  <si>
+    <t>https://imgur.com/S9MfqFY</t>
+  </si>
+  <si>
+    <t>https://imgur.com/c6GvlDw</t>
+  </si>
+  <si>
+    <t>https://imgur.com/lbcwNta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://imgur.com/4LvbvcB </t>
+  </si>
+  <si>
+    <t>https://imgur.com/36t79ym</t>
+  </si>
+  <si>
+    <t>https://imgur.com/mtwREAT</t>
+  </si>
+  <si>
+    <t>https://imgur.com/mUvbhQv</t>
+  </si>
+  <si>
+    <t>https://imgur.com/5RoySNu</t>
+  </si>
+  <si>
+    <t>https://imgur.com/Oosbzc4</t>
+  </si>
+  <si>
+    <t>https://imgur.com/HrMrPJS</t>
+  </si>
+  <si>
+    <t>https://imgur.com/6kcZeHL</t>
+  </si>
+  <si>
+    <t>https://imgur.com/mBR56k3</t>
+  </si>
+  <si>
+    <t>https://imgur.com/DCXIUy0</t>
+  </si>
+  <si>
+    <t>https://imgur.com/4F6s6gC</t>
+  </si>
+  <si>
+    <t>https://imgur.com/PmqWTqN</t>
+  </si>
+  <si>
+    <t>https://imgur.com/PXKDzo2</t>
+  </si>
+  <si>
+    <t>https://imgur.com/XJGbTRS</t>
+  </si>
+  <si>
+    <t>https://imgur.com/oMHzmMy</t>
+  </si>
+  <si>
+    <t>https://imgur.com/SIUYr5R</t>
+  </si>
+  <si>
+    <t>https://imgur.com/SIV6pDh</t>
+  </si>
+  <si>
+    <t>https://imgur.com/tAwIe0w</t>
+  </si>
+  <si>
+    <t>https://imgur.com/KMOuIVt</t>
+  </si>
+  <si>
+    <t>https://imgur.com/ZQb3X2i</t>
+  </si>
+  <si>
+    <t>https://imgur.com/CfYV3Qk</t>
+  </si>
+  <si>
+    <t>https://imgur.com/6xxmFES</t>
+  </si>
+  <si>
+    <t>https://imgur.com/iAtAikc</t>
+  </si>
+  <si>
+    <t>https://imgur.com/1ITNHEv</t>
+  </si>
+  <si>
+    <t>https://imgur.com/OobvCWF</t>
+  </si>
+  <si>
+    <t>https://imgur.com/Z7QJDZt</t>
+  </si>
+  <si>
+    <t>https://imgur.com/upaIlm9</t>
+  </si>
+  <si>
+    <t>https://imgur.com/xl92lVa</t>
+  </si>
+  <si>
+    <t>https://imgur.com/aRNYjCO</t>
+  </si>
+  <si>
+    <t>https://imgur.com/EYVTSgQ</t>
+  </si>
+  <si>
+    <t>https://imgur.com/GIZJDzE</t>
+  </si>
+  <si>
+    <t>https://imgur.com/85vcA7l</t>
+  </si>
+  <si>
+    <t>https://imgur.com/lPNGfDu</t>
+  </si>
+  <si>
+    <t>idk</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,22 +3154,22 @@
         <v>123</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>281</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>53</v>
       </c>
       <c r="J46" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K46" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="K46" s="14" t="s">
-        <v>284</v>
       </c>
       <c r="L46" s="13"/>
     </row>
@@ -3066,10 +3183,14 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+      <c r="H47" s="3" t="s">
+        <v>326</v>
+      </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="14"/>
+      <c r="K47" s="14" t="s">
+        <v>288</v>
+      </c>
       <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3085,7 +3206,9 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="14"/>
+      <c r="K48" s="14" t="s">
+        <v>289</v>
+      </c>
       <c r="L48" s="13"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3101,7 +3224,9 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="14"/>
+      <c r="K49" s="14" t="s">
+        <v>290</v>
+      </c>
       <c r="L49" s="13"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3117,7 +3242,9 @@
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="14"/>
+      <c r="K50" s="14" t="s">
+        <v>291</v>
+      </c>
       <c r="L50" s="13"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3133,7 +3260,9 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="14"/>
+      <c r="K51" s="14" t="s">
+        <v>292</v>
+      </c>
       <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3149,7 +3278,9 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="14"/>
+      <c r="K52" s="14" t="s">
+        <v>293</v>
+      </c>
       <c r="L52" s="13"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3165,7 +3296,9 @@
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="14"/>
+      <c r="K53" s="14" t="s">
+        <v>294</v>
+      </c>
       <c r="L53" s="13"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3181,7 +3314,9 @@
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="14"/>
+      <c r="K54" s="14" t="s">
+        <v>295</v>
+      </c>
       <c r="L54" s="13"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3197,7 +3332,9 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="14"/>
+      <c r="K55" s="14" t="s">
+        <v>296</v>
+      </c>
       <c r="L55" s="13"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3213,7 +3350,9 @@
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="14"/>
+      <c r="K56" s="14" t="s">
+        <v>297</v>
+      </c>
       <c r="L56" s="13"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3229,7 +3368,9 @@
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="14"/>
+      <c r="K57" s="14" t="s">
+        <v>298</v>
+      </c>
       <c r="L57" s="13"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3245,7 +3386,9 @@
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="14"/>
+      <c r="K58" s="14" t="s">
+        <v>299</v>
+      </c>
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3261,7 +3404,9 @@
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="14"/>
+      <c r="K59" s="14" t="s">
+        <v>300</v>
+      </c>
       <c r="L59" s="13"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -3277,7 +3422,9 @@
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="14"/>
+      <c r="K60" s="14" t="s">
+        <v>301</v>
+      </c>
       <c r="L60" s="13"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3293,7 +3440,9 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="14"/>
+      <c r="K61" s="14" t="s">
+        <v>302</v>
+      </c>
       <c r="L61" s="13"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -3309,7 +3458,9 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="14"/>
+      <c r="K62" s="14" t="s">
+        <v>303</v>
+      </c>
       <c r="L62" s="13"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3325,7 +3476,9 @@
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
-      <c r="K63" s="14"/>
+      <c r="K63" s="14" t="s">
+        <v>304</v>
+      </c>
       <c r="L63" s="13"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3341,7 +3494,9 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="14"/>
+      <c r="K64" s="14" t="s">
+        <v>305</v>
+      </c>
       <c r="L64" s="13"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3357,7 +3512,9 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
-      <c r="K65" s="14"/>
+      <c r="K65" s="14" t="s">
+        <v>306</v>
+      </c>
       <c r="L65" s="13"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3373,7 +3530,9 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
-      <c r="K66" s="14"/>
+      <c r="K66" s="14" t="s">
+        <v>307</v>
+      </c>
       <c r="L66" s="13"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3389,7 +3548,9 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-      <c r="K67" s="14"/>
+      <c r="K67" s="14" t="s">
+        <v>308</v>
+      </c>
       <c r="L67" s="13"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3405,7 +3566,9 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-      <c r="K68" s="14"/>
+      <c r="K68" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="L68" s="13"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3421,7 +3584,9 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-      <c r="K69" s="14"/>
+      <c r="K69" s="14" t="s">
+        <v>310</v>
+      </c>
       <c r="L69" s="13"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3437,7 +3602,9 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-      <c r="K70" s="14"/>
+      <c r="K70" s="14" t="s">
+        <v>311</v>
+      </c>
       <c r="L70" s="13"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3453,7 +3620,9 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
-      <c r="K71" s="14"/>
+      <c r="K71" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="L71" s="13"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3469,7 +3638,9 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="14"/>
+      <c r="K72" s="14" t="s">
+        <v>313</v>
+      </c>
       <c r="L72" s="13"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3485,7 +3656,9 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="14"/>
+      <c r="K73" s="14" t="s">
+        <v>314</v>
+      </c>
       <c r="L73" s="13"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3501,7 +3674,9 @@
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
-      <c r="K74" s="14"/>
+      <c r="K74" s="14" t="s">
+        <v>315</v>
+      </c>
       <c r="L74" s="13"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3517,7 +3692,9 @@
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
-      <c r="K75" s="14"/>
+      <c r="K75" s="14" t="s">
+        <v>316</v>
+      </c>
       <c r="L75" s="13"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3533,7 +3710,9 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="14"/>
+      <c r="K76" s="14" t="s">
+        <v>317</v>
+      </c>
       <c r="L76" s="13"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3549,7 +3728,9 @@
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
-      <c r="K77" s="14"/>
+      <c r="K77" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="L77" s="13"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3565,7 +3746,9 @@
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
-      <c r="K78" s="14"/>
+      <c r="K78" s="14" t="s">
+        <v>319</v>
+      </c>
       <c r="L78" s="13"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3581,8 +3764,180 @@
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-      <c r="K79" s="14"/>
+      <c r="K79" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="L79" s="13"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="L80" s="13"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="L81" s="13"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="L82" s="13"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="L83" s="13"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="L84" s="13"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="13"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="13"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>86</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="13"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>87</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="13"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3631,9 +3986,47 @@
     <hyperlink ref="K45" r:id="rId43"/>
     <hyperlink ref="K44" r:id="rId44"/>
     <hyperlink ref="K46" r:id="rId45"/>
+    <hyperlink ref="K47" r:id="rId46"/>
+    <hyperlink ref="K48" r:id="rId47"/>
+    <hyperlink ref="K49" r:id="rId48"/>
+    <hyperlink ref="K50" r:id="rId49"/>
+    <hyperlink ref="K51" r:id="rId50"/>
+    <hyperlink ref="K52" r:id="rId51"/>
+    <hyperlink ref="K53" r:id="rId52"/>
+    <hyperlink ref="K54" r:id="rId53"/>
+    <hyperlink ref="K55" r:id="rId54"/>
+    <hyperlink ref="K56" r:id="rId55"/>
+    <hyperlink ref="K57" r:id="rId56"/>
+    <hyperlink ref="K58" r:id="rId57"/>
+    <hyperlink ref="K59" r:id="rId58"/>
+    <hyperlink ref="K60" r:id="rId59"/>
+    <hyperlink ref="K61" r:id="rId60"/>
+    <hyperlink ref="K62" r:id="rId61"/>
+    <hyperlink ref="K63" r:id="rId62"/>
+    <hyperlink ref="K64" r:id="rId63"/>
+    <hyperlink ref="K65" r:id="rId64"/>
+    <hyperlink ref="K66" r:id="rId65"/>
+    <hyperlink ref="K67" r:id="rId66"/>
+    <hyperlink ref="K68" r:id="rId67"/>
+    <hyperlink ref="K69" r:id="rId68"/>
+    <hyperlink ref="K70" r:id="rId69"/>
+    <hyperlink ref="K71" r:id="rId70"/>
+    <hyperlink ref="K72" r:id="rId71"/>
+    <hyperlink ref="K73" r:id="rId72"/>
+    <hyperlink ref="K74" r:id="rId73"/>
+    <hyperlink ref="K75" r:id="rId74"/>
+    <hyperlink ref="K76" r:id="rId75"/>
+    <hyperlink ref="K77" r:id="rId76"/>
+    <hyperlink ref="K78" r:id="rId77"/>
+    <hyperlink ref="K79" r:id="rId78"/>
+    <hyperlink ref="K80" r:id="rId79"/>
+    <hyperlink ref="K81" r:id="rId80"/>
+    <hyperlink ref="K82" r:id="rId81"/>
+    <hyperlink ref="K83" r:id="rId82"/>
+    <hyperlink ref="K84" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId84"/>
 </worksheet>
 </file>
 

</xml_diff>